<commit_message>
Update descriptive statistics for ELB and MAR weather datasets
</commit_message>
<xml_diff>
--- a/Descriptive_Statistics_MAR.xlsx
+++ b/Descriptive_Statistics_MAR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,695 +434,716 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>This is the original case study area MAR.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>It includes quantitative and qualitative groundwater data for 10 monitoring sites.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>There are 20 different parameters measured. In total, there are 830 groundwater samples with over 1,400 individual datapoints.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>count</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>mean</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>std</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>min</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>50%</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>75%</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>max</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>ABSTICH m</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>690</v>
-      </c>
-      <c r="C2" t="n">
-        <v>5.205942028985507</v>
-      </c>
-      <c r="D2" t="n">
-        <v>38.36889780130777</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.6725</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4.72</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>NITRAT mg/l</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>764</v>
-      </c>
-      <c r="C3" t="n">
-        <v>26.95969895287958</v>
-      </c>
-      <c r="D3" t="n">
-        <v>15.02387595038057</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>19.1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>27.55</v>
-      </c>
-      <c r="H3" t="n">
-        <v>35.7</v>
-      </c>
-      <c r="I3" t="n">
-        <v>88.59999999999999</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>DOC mg/l</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>777</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2.085237323037323</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.564580012046328</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="I4" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>KALIUM mg/l</t>
+          <t>ABSTICH m</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>789</v>
+        <v>690</v>
       </c>
       <c r="C5" t="n">
-        <v>8.653227490494297</v>
+        <v>5.205942028985507</v>
       </c>
       <c r="D5" t="n">
-        <v>11.99605223829685</v>
+        <v>38.36889780130777</v>
       </c>
       <c r="E5" t="n">
-        <v>0.38</v>
+        <v>0.25</v>
       </c>
       <c r="F5" t="n">
-        <v>2.4</v>
+        <v>1.6725</v>
       </c>
       <c r="G5" t="n">
-        <v>3.88</v>
+        <v>3.7</v>
       </c>
       <c r="H5" t="n">
-        <v>9.199999999999999</v>
+        <v>4.72</v>
       </c>
       <c r="I5" t="n">
-        <v>67.3</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>LFD. NUMMER.</t>
+          <t>NITRAT mg/l</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>805</v>
+        <v>764</v>
       </c>
       <c r="C6" t="n">
-        <v>31666426.63354037</v>
+        <v>26.95969895287958</v>
       </c>
       <c r="D6" t="n">
-        <v>597123.121182739</v>
+        <v>15.02387595038057</v>
       </c>
       <c r="E6" t="n">
-        <v>31000292</v>
+        <v>0.2</v>
       </c>
       <c r="F6" t="n">
-        <v>31100302</v>
+        <v>19.1</v>
       </c>
       <c r="G6" t="n">
-        <v>31100322</v>
+        <v>27.55</v>
       </c>
       <c r="H6" t="n">
-        <v>32200092</v>
+        <v>35.7</v>
       </c>
       <c r="I6" t="n">
-        <v>32500392</v>
+        <v>88.59999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>ORTHOPHOSPHAT mg/l</t>
+          <t>DOC mg/l</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>809</v>
+        <v>777</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3911273176761434</v>
+        <v>2.085237323037323</v>
       </c>
       <c r="D7" t="n">
-        <v>0.520284227784236</v>
+        <v>1.564580012046328</v>
       </c>
       <c r="E7" t="n">
-        <v>0.011</v>
+        <v>0.42</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="G7" t="n">
-        <v>0.172</v>
+        <v>1.5</v>
       </c>
       <c r="H7" t="n">
-        <v>0.476</v>
+        <v>2.99</v>
       </c>
       <c r="I7" t="n">
-        <v>4.49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>SAUERSTOFFGEHALT mg/l</t>
+          <t>KALIUM mg/l</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>813</v>
+        <v>789</v>
       </c>
       <c r="C8" t="n">
-        <v>5.16769987699877</v>
+        <v>8.653227490494297</v>
       </c>
       <c r="D8" t="n">
-        <v>2.903766663477565</v>
+        <v>11.99605223829685</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="F8" t="n">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="G8" t="n">
-        <v>5</v>
+        <v>3.88</v>
       </c>
       <c r="H8" t="n">
-        <v>7.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>13.1</v>
+        <v>67.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>LUFTTEMPERATUR IN °C</t>
+          <t>LFD. NUMMER.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="C9" t="n">
-        <v>13.1963144963145</v>
+        <v>31666426.63354037</v>
       </c>
       <c r="D9" t="n">
-        <v>8.526495060203313</v>
+        <v>597123.121182739</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.199999999999999</v>
+        <v>31000292</v>
       </c>
       <c r="F9" t="n">
-        <v>7</v>
+        <v>31100302</v>
       </c>
       <c r="G9" t="n">
-        <v>13</v>
+        <v>31100322</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
+        <v>32200092</v>
       </c>
       <c r="I9" t="n">
-        <v>36</v>
+        <v>32500392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>KARBONATHAERTE °dH</t>
+          <t>ORTHOPHOSPHAT mg/l</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>825</v>
+        <v>809</v>
       </c>
       <c r="C10" t="n">
-        <v>8.580953696969697</v>
+        <v>0.3911273176761434</v>
       </c>
       <c r="D10" t="n">
-        <v>3.40351387848041</v>
+        <v>0.520284227784236</v>
       </c>
       <c r="E10" t="n">
-        <v>2.7</v>
+        <v>0.011</v>
       </c>
       <c r="F10" t="n">
-        <v>5.68</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>8.199999999999999</v>
+        <v>0.172</v>
       </c>
       <c r="H10" t="n">
-        <v>11.4</v>
+        <v>0.476</v>
       </c>
       <c r="I10" t="n">
-        <v>21.2</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>HYDROGENK. mg/l</t>
+          <t>SAUERSTOFFGEHALT mg/l</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>825</v>
+        <v>813</v>
       </c>
       <c r="C11" t="n">
-        <v>186.6351224242424</v>
+        <v>5.16769987699877</v>
       </c>
       <c r="D11" t="n">
-        <v>74.1377754573396</v>
+        <v>2.903766663477565</v>
       </c>
       <c r="E11" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>123</v>
+        <v>2.8</v>
       </c>
       <c r="G11" t="n">
-        <v>178.7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="n">
-        <v>248</v>
+        <v>7.8</v>
       </c>
       <c r="I11" t="n">
-        <v>462</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>MAGNESIUM mg/l</t>
+          <t>LUFTTEMPERATUR IN °C</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>829</v>
+        <v>814</v>
       </c>
       <c r="C12" t="n">
-        <v>16.03845644149578</v>
+        <v>13.1963144963145</v>
       </c>
       <c r="D12" t="n">
-        <v>5.628175442803776</v>
+        <v>8.526495060203313</v>
       </c>
       <c r="E12" t="n">
-        <v>7.48</v>
+        <v>-9.199999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>11.8</v>
+        <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>15.1</v>
+        <v>13</v>
       </c>
       <c r="H12" t="n">
-        <v>19.6</v>
+        <v>20</v>
       </c>
       <c r="I12" t="n">
-        <v>34.6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>NATRIUM mg/l</t>
+          <t>KARBONATHAERTE °dH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="C13" t="n">
-        <v>11.32994446320868</v>
+        <v>8.580953696969697</v>
       </c>
       <c r="D13" t="n">
-        <v>3.533391998667081</v>
+        <v>3.40351387848041</v>
       </c>
       <c r="E13" t="n">
-        <v>5.2</v>
+        <v>2.7</v>
       </c>
       <c r="F13" t="n">
-        <v>9.1</v>
+        <v>5.68</v>
       </c>
       <c r="G13" t="n">
-        <v>10.6</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>12.5</v>
+        <v>11.4</v>
       </c>
       <c r="I13" t="n">
-        <v>36.1</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>CALCIUM mg/l</t>
+          <t>HYDROGENK. mg/l</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="C14" t="n">
-        <v>62.6861723039807</v>
+        <v>186.6351224242424</v>
       </c>
       <c r="D14" t="n">
-        <v>23.13164214482053</v>
+        <v>74.1377754573396</v>
       </c>
       <c r="E14" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="F14" t="n">
-        <v>42.9</v>
+        <v>123</v>
       </c>
       <c r="G14" t="n">
-        <v>59.5</v>
+        <v>178.7</v>
       </c>
       <c r="H14" t="n">
-        <v>79.8</v>
+        <v>248</v>
       </c>
       <c r="I14" t="n">
-        <v>134.8</v>
+        <v>462</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>E-UHRZEIT</t>
+          <t>MAGNESIUM mg/l</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>829</v>
       </c>
       <c r="C15" t="n">
-        <v>31.37435464414958</v>
+        <v>16.03845644149578</v>
       </c>
       <c r="D15" t="n">
-        <v>517.596333403856</v>
+        <v>5.628175442803776</v>
       </c>
       <c r="E15" t="n">
-        <v>7.2</v>
+        <v>7.48</v>
       </c>
       <c r="F15" t="n">
-        <v>11.2</v>
+        <v>11.8</v>
       </c>
       <c r="G15" t="n">
-        <v>13.41</v>
+        <v>15.1</v>
       </c>
       <c r="H15" t="n">
-        <v>15.35</v>
+        <v>19.6</v>
       </c>
       <c r="I15" t="n">
-        <v>14916</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>GESAMTHAERTE °dH</t>
+          <t>NATRIUM mg/l</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>829</v>
       </c>
       <c r="C16" t="n">
-        <v>12.46677416164053</v>
+        <v>11.32994446320868</v>
       </c>
       <c r="D16" t="n">
-        <v>4.39451108230128</v>
+        <v>3.533391998667081</v>
       </c>
       <c r="E16" t="n">
-        <v>5.14</v>
+        <v>5.2</v>
       </c>
       <c r="F16" t="n">
-        <v>8.800000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="G16" t="n">
-        <v>11.7</v>
+        <v>10.6</v>
       </c>
       <c r="H16" t="n">
-        <v>16</v>
+        <v>12.5</v>
       </c>
       <c r="I16" t="n">
-        <v>25.4</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>ELEKTR. LEITF. (bei 20°C) µS/cm</t>
+          <t>CALCIUM mg/l</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>829</v>
       </c>
       <c r="C17" t="n">
-        <v>463.2125638600724</v>
+        <v>62.6861723039807</v>
       </c>
       <c r="D17" t="n">
-        <v>149.5555538435822</v>
+        <v>23.13164214482053</v>
       </c>
       <c r="E17" t="n">
-        <v>159.49821</v>
+        <v>23</v>
       </c>
       <c r="F17" t="n">
-        <v>353</v>
+        <v>42.9</v>
       </c>
       <c r="G17" t="n">
-        <v>432.7957</v>
+        <v>59.5</v>
       </c>
       <c r="H17" t="n">
-        <v>578</v>
+        <v>79.8</v>
       </c>
       <c r="I17" t="n">
-        <v>1033.15412</v>
+        <v>134.8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>CHLORID mg/l</t>
+          <t>E-UHRZEIT</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>829</v>
       </c>
       <c r="C18" t="n">
-        <v>31.902958986731</v>
+        <v>31.37435464414958</v>
       </c>
       <c r="D18" t="n">
-        <v>17.64527256681668</v>
+        <v>517.596333403856</v>
       </c>
       <c r="E18" t="n">
-        <v>5.1</v>
+        <v>7.2</v>
       </c>
       <c r="F18" t="n">
-        <v>17.2</v>
+        <v>11.2</v>
       </c>
       <c r="G18" t="n">
-        <v>28.1</v>
+        <v>13.41</v>
       </c>
       <c r="H18" t="n">
-        <v>44</v>
+        <v>15.35</v>
       </c>
       <c r="I18" t="n">
-        <v>108</v>
+        <v>14916</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>SULFAT mg/l</t>
+          <t>GESAMTHAERTE °dH</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>829</v>
       </c>
       <c r="C19" t="n">
-        <v>41.10123763570567</v>
+        <v>12.46677416164053</v>
       </c>
       <c r="D19" t="n">
-        <v>17.44302922463943</v>
+        <v>4.39451108230128</v>
       </c>
       <c r="E19" t="n">
-        <v>5.97</v>
+        <v>5.14</v>
       </c>
       <c r="F19" t="n">
-        <v>27.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G19" t="n">
-        <v>38.3</v>
+        <v>11.7</v>
       </c>
       <c r="H19" t="n">
-        <v>51.5</v>
+        <v>16</v>
       </c>
       <c r="I19" t="n">
-        <v>121.7</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>ELEKTR. LEITF. (bei 25°C) µS/cm</t>
+          <t>ELEKTR. LEITF. (bei 20°C) µS/cm</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>829</v>
       </c>
       <c r="C20" t="n">
-        <v>516.9427074547648</v>
+        <v>463.2125638600724</v>
       </c>
       <c r="D20" t="n">
-        <v>166.9020150827988</v>
+        <v>149.5555538435822</v>
       </c>
       <c r="E20" t="n">
-        <v>178</v>
+        <v>159.49821</v>
       </c>
       <c r="F20" t="n">
-        <v>393.948</v>
+        <v>353</v>
       </c>
       <c r="G20" t="n">
-        <v>483</v>
+        <v>432.7957</v>
       </c>
       <c r="H20" t="n">
-        <v>645.048</v>
+        <v>578</v>
       </c>
       <c r="I20" t="n">
-        <v>1153</v>
+        <v>1033.15412</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>PH-WERT</t>
+          <t>CHLORID mg/l</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C21" t="n">
-        <v>7.078048192771085</v>
+        <v>31.902958986731</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2678341809006692</v>
+        <v>17.64527256681668</v>
       </c>
       <c r="E21" t="n">
-        <v>5.99</v>
+        <v>5.1</v>
       </c>
       <c r="F21" t="n">
-        <v>6.9</v>
+        <v>17.2</v>
       </c>
       <c r="G21" t="n">
-        <v>7.1</v>
+        <v>28.1</v>
       </c>
       <c r="H21" t="n">
-        <v>7.3</v>
+        <v>44</v>
       </c>
       <c r="I21" t="n">
-        <v>8.43</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
+          <t>SULFAT mg/l</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>829</v>
+      </c>
+      <c r="C22" t="n">
+        <v>41.10123763570567</v>
+      </c>
+      <c r="D22" t="n">
+        <v>17.44302922463943</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="F22" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="H22" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>121.7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>ELEKTR. LEITF. (bei 25°C) µS/cm</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>829</v>
+      </c>
+      <c r="C23" t="n">
+        <v>516.9427074547648</v>
+      </c>
+      <c r="D23" t="n">
+        <v>166.9020150827988</v>
+      </c>
+      <c r="E23" t="n">
+        <v>178</v>
+      </c>
+      <c r="F23" t="n">
+        <v>393.948</v>
+      </c>
+      <c r="G23" t="n">
+        <v>483</v>
+      </c>
+      <c r="H23" t="n">
+        <v>645.048</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>PH-WERT</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>830</v>
+      </c>
+      <c r="C24" t="n">
+        <v>7.078048192771085</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.2678341809006692</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="F24" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="I24" t="n">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
           <t>WASSERTEMPERATUR °C</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B25" t="n">
         <v>830</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C25" t="n">
         <v>10.20771084337349</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D25" t="n">
         <v>2.211389165056073</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E25" t="n">
         <v>2.6</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F25" t="n">
         <v>9</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G25" t="n">
         <v>10.1</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H25" t="n">
         <v>11.5</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I25" t="n">
         <v>17.2</v>
       </c>
     </row>

</xml_diff>